<commit_message>
Demonstration, including unit testing
</commit_message>
<xml_diff>
--- a/tests/M01_demonstration_test_plan_course.xlsx
+++ b/tests/M01_demonstration_test_plan_course.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\3. Demonstrations\module_1\requirements_document\given_files\isd_demonstration\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ralph\OneDrive - Red River College Polytech\Desktop\Intermidiate_Software_Development\Demonstration\Student\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023FC87A-C2C8-4B8F-9C8F-59EA44F44E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E58F68F-B9B8-4F3B-986C-73CBD15E9334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="8230" yWindow="410" windowWidth="15180" windowHeight="11870" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -255,6 +255,18 @@
   </si>
   <si>
     <t>Course</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>name="ISD" department=COMPUTER_SCIENCE credit_hours=6</t>
+  </si>
+  <si>
+    <t>Client object created with expected attribute values</t>
+  </si>
+  <si>
+    <t>ValueError</t>
   </si>
 </sst>
 </file>
@@ -529,6 +541,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -552,12 +570,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1115,53 +1127,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C5" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="6" max="6" width="35.453125" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.15">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="16"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1181,9 +1193,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
-      <c r="B7" s="19">
+      <c r="B7" s="11">
         <v>1</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -1192,13 +1204,19 @@
       <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
-      <c r="B8" s="20">
+      <c r="B8" s="12">
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1207,13 +1225,19 @@
       <c r="D8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
-      <c r="B9" s="20">
+      <c r="B9" s="12">
         <v>3</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1226,9 +1250,9 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
-      <c r="B10" s="19">
+      <c r="B10" s="11">
         <v>4</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -1241,8 +1265,8 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20">
+    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="12">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1255,8 +1279,8 @@
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20">
+    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="12">
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1269,8 +1293,8 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="19">
+    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="11">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1283,8 +1307,8 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20">
+    <row r="14" spans="1:7" ht="96.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="12">
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1297,8 +1321,8 @@
       <c r="F14" s="3"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="20">
+    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="12">
         <v>9</v>
       </c>
       <c r="C15" s="3"/>
@@ -1307,8 +1331,8 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="19">
+    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="11">
         <v>10</v>
       </c>
       <c r="C16" s="3"/>
@@ -1317,8 +1341,8 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="20">
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="12">
         <v>11</v>
       </c>
       <c r="C17" s="3"/>
@@ -1327,8 +1351,8 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="20">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="12">
         <v>12</v>
       </c>
       <c r="C18" s="3"/>
@@ -1337,8 +1361,8 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="19">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="11">
         <v>13</v>
       </c>
       <c r="C19" s="3"/>
@@ -1347,8 +1371,8 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="12">
         <v>14</v>
       </c>
       <c r="C20" s="3"/>
@@ -1357,8 +1381,8 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="12">
         <v>15</v>
       </c>
       <c r="C21" s="3"/>
@@ -1367,8 +1391,8 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="19">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="11">
         <v>16</v>
       </c>
       <c r="C22" s="3"/>
@@ -1377,8 +1401,8 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="20">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="12">
         <v>17</v>
       </c>
       <c r="C23" s="3"/>
@@ -1387,8 +1411,8 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20">
+    <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="12">
         <v>18</v>
       </c>
       <c r="C24" s="3"/>
@@ -1397,8 +1421,8 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="19">
+    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="11">
         <v>19</v>
       </c>
       <c r="C25" s="3"/>
@@ -1407,8 +1431,8 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="20">
+    <row r="26" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="12">
         <v>20</v>
       </c>
       <c r="C26" s="3"/>
@@ -1417,15 +1441,15 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="17" t="s">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1443,6 +1467,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003B3B6B51C940774DBF92367B1D1A75F0" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80d4f13eaa95653e2ff902bb880fefc3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee0e594b-5dc6-49aa-9be8-f17bb89b127c" xmlns:ns3="b80edf0c-bd47-4bae-8c19-89fc2af9398f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ababe2f621e4b192c84b1cec6edec4f" ns2:_="" ns3:_="">
     <xsd:import namespace="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
@@ -1637,15 +1670,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1658,13 +1682,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D37D0E6-97E2-42C6-8F1C-5D374F1DFD51}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{478BB3D1-82ED-4256-B1E3-83928DEEA9DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{478BB3D1-82ED-4256-B1E3-83928DEEA9DA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D37D0E6-97E2-42C6-8F1C-5D374F1DFD51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
+    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C74A9BB-248F-4445-8C38-16C1F5CA6134}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C74A9BB-248F-4445-8C38-16C1F5CA6134}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
+    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>